<commit_message>
Add run functions to run MLP, Logistic Regression and Random Forest with best parameters with kFold training/testing split. Add results on falsely-classified instances by these models.
</commit_message>
<xml_diff>
--- a/Results/kfold-training-testing-split-results.xlsx
+++ b/Results/kfold-training-testing-split-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A790E111-8017-A745-B5FB-AB3AC2E462DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A694A0-D50E-3B43-ACDB-FEFFE026F74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D7CE87F8-77C2-F944-904B-08A0D09A1FAF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>1st Fold Accuracy</t>
   </si>
@@ -58,101 +58,6 @@
   </si>
   <si>
     <t>Note:</t>
-  </si>
-  <si>
-    <t>Underscored parameters are those being tuned by a Grid Search. Each of the candidates are trained and we select the one that generates the best accuracy.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Multi-layer Perceptron
-    Photons Histogramizer: 6 buckets, filter late-arrival photons
-    MLP: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4 hidden layers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>8-40</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> neurons per layer</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Multi-layer Perceptron
-    Photons Histogramizer: 6 buckets, filter late-arrival photons
-    MLP: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2 hidden layers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">8-40 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>neurons per layer</t>
-    </r>
   </si>
   <si>
     <r>
@@ -198,7 +103,215 @@
     <t>5 histogram buckets</t>
   </si>
   <si>
-    <t>Threshold value for "late-arrival phtoons": have performed grid search on Max's previous empirical value and Aaron's value shown by the histogram of all phtons' arrival times. Performance difference is insignificant.</t>
+    <t>15 neurons per layer</t>
+  </si>
+  <si>
+    <t>39 neurons per layer</t>
+  </si>
+  <si>
+    <t>10 neurons per layer</t>
+  </si>
+  <si>
+    <t>24 neurons per layer</t>
+  </si>
+  <si>
+    <t>36 neurons per layer</t>
+  </si>
+  <si>
+    <t>28 neurons per layer</t>
+  </si>
+  <si>
+    <t>22 neurons per layer</t>
+  </si>
+  <si>
+    <t>31 neurons per layer</t>
+  </si>
+  <si>
+    <t>29 neurons per layer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multi-layer Perceptron
+    Photons Histogramizer: 6 buckets, filter late-arrival photons </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(BEST, POST_THRESHOLD)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    MLP: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 hidden layers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">8-40 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>neurons per layer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multi-layer Perceptron
+    Photons Histogramizer: 6 buckets, filter late-arrival photons </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(BEST, POST_THRESHOLD)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    MLP: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 hidden layers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>8-40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> neurons per layer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multi-layer Perceptron
+    Photons Histogramizer: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1-32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> buckets, filter late-arrival photons (POST_THRESHOLD)
+    MLP: 2 hidden layers, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>8-40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> neurons per layer</t>
+    </r>
+  </si>
+  <si>
+    <t>(Still running)</t>
+  </si>
+  <si>
+    <t>Threshold value for "late-arrival phtoons": have performed grid search on Max's previous empirical value (BEST) and Aaron's value (POST) shown by the histogram of all phtons' arrival times. Performance difference is insignificant.</t>
+  </si>
+  <si>
+    <t>Underscored parameters are those being tuned by a Grid Search. Each of the candidates is trained and we select the one that generates the best accuracy.</t>
   </si>
 </sst>
 </file>
@@ -586,24 +699,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31911894-FECC-5943-B840-F1C4CE52A234}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="73.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
     <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" customWidth="1"/>
     <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -632,149 +745,187 @@
     </row>
     <row r="2" spans="1:12">
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="66" customHeight="1">
+    <row r="3" spans="1:12" ht="102">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>0.99978043834837904</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
         <v>0.99965128443566198</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2">
         <v>0.99970294600074905</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2">
         <v>0.99957378658331797</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J3" s="2">
         <v>0.99975460439645603</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L3" s="2">
         <v>0.99969261195291304</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="51">
+    <row r="4" spans="1:12" ht="68">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>0.99978043834837904</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="2">
         <v>0.999664199826933</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="2">
         <v>0.99970294600074905</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H4" s="2">
         <v>0.99962544881564297</v>
       </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="2">
         <v>0.99978043551261797</v>
       </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
       <c r="L4" s="2">
         <v>0.99971069370086396</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="51">
+    <row r="5" spans="1:12" ht="68">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2">
         <v>0.99978043834837904</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="2">
         <v>0.999664199826933</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="2">
         <v>0.99970294600074905</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="2">
         <v>0.99961253325756205</v>
       </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
       <c r="J5" s="2">
         <v>0.99976751995453705</v>
       </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
       <c r="L5" s="2">
         <v>0.99970552747763197</v>
       </c>
     </row>
+    <row r="6" spans="1:12" ht="68">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.99970811064931098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.99970811064931098</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Summarize Week 7 KFold results and prepare talking to Jens: add MLP cross validation method that removes the extra layer of doing testing 5 times. Refactor script to graph histogram of all mis-classified qubits' photons.
</commit_message>
<xml_diff>
--- a/Results/kfold-training-testing-split-results.xlsx
+++ b/Results/kfold-training-testing-split-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/CS-Projects/Qubit-Capstone/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A694A0-D50E-3B43-ACDB-FEFFE026F74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00803F4-2DA3-EF46-B872-916DA2796C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D7CE87F8-77C2-F944-904B-08A0D09A1FAF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>1st Fold Accuracy</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>Underscored parameters are those being tuned by a Grid Search. Each of the candidates is trained and we select the one that generates the best accuracy.</t>
+  </si>
+  <si>
+    <t>{'clf__hidden_layer_sizes': (15, 15), 'hstgm__num_buckets': 4}</t>
+  </si>
+  <si>
+    <t>{'clf__hidden_layer_sizes': (13, 13), 'hstgm__num_buckets': 15}</t>
+  </si>
+  <si>
+    <t>{'clf__hidden_layer_sizes': (19, 19), 'hstgm__num_buckets': 6}</t>
+  </si>
+  <si>
+    <t>{'clf__hidden_layer_sizes': (20, 20), 'hstgm__num_buckets': 2}</t>
   </si>
 </sst>
 </file>
@@ -319,7 +331,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -375,15 +387,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,10 +714,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31911894-FECC-5943-B840-F1C4CE52A234}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -896,9 +914,34 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2">
+        <v>0.99971586139201996</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.99965128443566198</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.99971586139201996</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>0.999638364373724</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
         <v>26</v>
       </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
@@ -936,7 +979,8 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Code inspection on run_mlp_with_cross_validation_average (use params to generate results in Excel sheet), run_mlp_grid_search_cv_with_cross_validation_average (fix picklize failure). Add script to generate qubit bar chart by photons count.
</commit_message>
<xml_diff>
--- a/Results/kfold-training-testing-split-results.xlsx
+++ b/Results/kfold-training-testing-split-results.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/CS-Projects/Qubit-Capstone/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00803F4-2DA3-EF46-B872-916DA2796C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA89E96-997D-DC4E-A6DD-8455513F36F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D7CE87F8-77C2-F944-904B-08A0D09A1FAF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{D7CE87F8-77C2-F944-904B-08A0D09A1FAF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Separate Testing Method" sheetId="1" r:id="rId1"/>
+    <sheet name="Cross Validation Method" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>1st Fold Accuracy</t>
   </si>
@@ -324,6 +324,22 @@
   </si>
   <si>
     <t>{'clf__hidden_layer_sizes': (20, 20), 'hstgm__num_buckets': 2}</t>
+  </si>
+  <si>
+    <t>Model and Parameters</t>
+  </si>
+  <si>
+    <t>5-fold Cross Validation with averaged Accuracy, with New Data Split</t>
+  </si>
+  <si>
+    <t>MLPClassifier:
+  Layers (8-40, 8-40), 6 bins</t>
+  </si>
+  <si>
+    <t>Best Parameter</t>
+  </si>
+  <si>
+    <t>Layers (33, 33)</t>
   </si>
 </sst>
 </file>
@@ -394,11 +410,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,7 +735,7 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -740,26 +756,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:12">
       <c r="B2" t="s">
@@ -917,19 +933,19 @@
       <c r="B6" s="2">
         <v>0.99971586139201996</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="2">
         <v>0.99965128443566198</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="2">
         <v>0.99971586139201996</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H6">
@@ -986,12 +1002,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3979B56-16DF-2248-8563-45AECE0FAE48}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.99971585985737299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Materials for presentation on 02/28/2020 with UCLA Physics.
Generate overlap percentage of falsely-classified instances by different classifiers. Add code and generate plots for falsely-classified instances' qubits count VS. number of photons, photons' histograms for New Data Split.

Compute accuracies for grid searching params on the slides. Attempted Voting Classifier with New Data Split and get accuracy.
</commit_message>
<xml_diff>
--- a/Results/kfold-training-testing-split-results.xlsx
+++ b/Results/kfold-training-testing-split-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/CS-Projects/Qubit-Capstone/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA89E96-997D-DC4E-A6DD-8455513F36F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EA8006-A661-A24C-8931-9294BF1B6AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{D7CE87F8-77C2-F944-904B-08A0D09A1FAF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>1st Fold Accuracy</t>
   </si>
@@ -340,6 +340,30 @@
   </si>
   <si>
     <t>Layers (33, 33)</t>
+  </si>
+  <si>
+    <t>Majority Vote: 
+    mv_pipeline = Pipeline([
+        ('hstgm', Histogramize(
+            arrival_time_threshold=(PRE_ARRIVAL_TIME_THRESHOLD, POST_ARRIVAL_TIME_THRESHOLD))),
+        ('clf', VotingClassifier([
+            ('mlp', 
+                MLPClassifier(activation='relu', solver='adam', hidden_layer_sizes=(32, 32), random_state=RANDOM_SEED)),
+            ('tc', 
+                ThresholdCutoffClassifier(threshold=BEST_PHOTON_COUNT_THRESHOLD)),
+            ('lg', 
+                LogisticRegression(solver='liblinear', penalty='l2', C=10**-3, random_state=RANDOM_SEED)),
+            ('rf', 
+                RandomForestClassifier(random_state=RANDOM_SEED))
+        ]))
+    ])
+    mv_param_grid = {
+        'hstgm__num_buckets': range(5, 10),
+        'clf__mlp__hidden_layer_sizes': [(neurons,) * 2 for neurons in range(20, 41)],
+    }</t>
+  </si>
+  <si>
+    <t>(26, 26), 7</t>
   </si>
 </sst>
 </file>
@@ -1005,12 +1029,12 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="100" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
@@ -1037,6 +1061,17 @@
         <v>0.99971585985737299</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="356">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.99971840000000001</v>
+      </c>
+    </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>7</v>

</xml_diff>